<commit_message>
new change to cheak
</commit_message>
<xml_diff>
--- a/abcd.xlsx
+++ b/abcd.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\sarkari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9255E0E-86F6-4484-8D2C-191F5EF0743C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B62897-5DEC-4CE9-87CA-F03207C60AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{78020E63-11DB-4325-B747-9223D9F25A32}"/>
   </bookViews>
@@ -141,7 +141,7 @@
     <t>verify the password strength</t>
   </si>
   <si>
-    <t>v</t>
+    <t>new change to chck origin</t>
   </si>
 </sst>
 </file>
@@ -685,7 +685,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D22" s="1" t="s">
         <v>34</v>
       </c>

</xml_diff>